<commit_message>
feat(routes): added all routes to the routes file
</commit_message>
<xml_diff>
--- a/Documentation/routes-a-faire.xlsx
+++ b/Documentation/routes-a-faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\P_DEV_UNESCO\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62904B1F-706B-4E50-B91C-7EBCE258EFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34BFFA8-59B2-4EE9-B1D6-FD1E9063450C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>ROUTES</t>
   </si>
@@ -104,21 +104,12 @@
     <t>register</t>
   </si>
   <si>
-    <t>/register</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
-    <t>/login</t>
-  </si>
-  <si>
     <t>logout</t>
   </si>
   <si>
-    <t>/logout</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -152,12 +143,6 @@
     <t>/sites/id/saves</t>
   </si>
   <si>
-    <t>all users</t>
-  </si>
-  <si>
-    <t>user_fk, site_fk</t>
-  </si>
-  <si>
     <t>visite</t>
   </si>
   <si>
@@ -189,6 +174,21 @@
   </si>
   <si>
     <t>/countries</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
+    <t>/user/logout</t>
+  </si>
+  <si>
+    <t>/user/register</t>
+  </si>
+  <si>
+    <t>BONUS</t>
+  </si>
+  <si>
+    <t>date_visite</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +222,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -247,7 +253,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,13 +535,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S28"/>
+  <dimension ref="B2:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -548,7 +555,10 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -568,7 +578,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -576,7 +586,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
@@ -588,7 +598,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -604,7 +614,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -620,23 +630,23 @@
         <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -645,7 +655,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>17</v>
@@ -654,13 +664,10 @@
         <v>3</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -671,7 +678,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>14</v>
@@ -679,7 +686,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
@@ -688,13 +695,13 @@
         <v>3</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -705,70 +712,73 @@
         <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="6" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="2"/>
@@ -778,16 +788,16 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="2"/>
@@ -796,6 +806,18 @@
       <c r="S20" s="2"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -803,21 +825,6 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
@@ -825,6 +832,21 @@
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -832,79 +854,82 @@
       <c r="S23" s="2"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C27" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C28" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="F28" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>33</v>
+      <c r="G29" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(controllers): most of the controllers are working, still needs to work on sitesController
</commit_message>
<xml_diff>
--- a/Documentation/routes-a-faire.xlsx
+++ b/Documentation/routes-a-faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\P_DEV_UNESCO\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34BFFA8-59B2-4EE9-B1D6-FD1E9063450C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD524D8D-6E34-4169-A84C-B47FC8E29B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="B2:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,16 +588,16 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="2"/>
@@ -768,16 +768,16 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O19" s="1"/>
@@ -787,16 +787,16 @@
       <c r="S19" s="2"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O20" s="1"/>
@@ -806,16 +806,16 @@
       <c r="S20" s="2"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O21" s="1"/>

</xml_diff>